<commit_message>
* Move fixed formula test out ignored test class. * update formula test excel file. * Upgrade org.apache.common.math to 2.2
</commit_message>
<xml_diff>
--- a/zss.test/src/test/java/org/zkoss/zss/api/impl/book/TestFile2007-Formula.xlsx
+++ b/zss.test/src/test/java/org/zkoss/zss/api/impl/book/TestFile2007-Formula.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="18195" windowHeight="6885" firstSheet="7" activeTab="12"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="18195" windowHeight="6840" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="first-error" sheetId="12" r:id="rId1"/>
@@ -1428,7 +1428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="465">
   <si>
     <t>name-range formula</t>
   </si>
@@ -2809,6 +2809,26 @@
   </si>
   <si>
     <t>T</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>T</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test for Cumulative = True</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>TDIST</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>T</t>
+    <phoneticPr fontId="12" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test for one tail</t>
     <phoneticPr fontId="12" type="noConversion"/>
   </si>
 </sst>
@@ -2816,7 +2836,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="7">
+  <numFmts count="9">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="&quot;NT$&quot;#,##0.00;[Red]\-&quot;NT$&quot;#,##0.00"/>
     <numFmt numFmtId="177" formatCode="0.0000"/>
@@ -2824,6 +2844,8 @@
     <numFmt numFmtId="179" formatCode="0.0%"/>
     <numFmt numFmtId="180" formatCode="0_ ;[Red]\-0\ "/>
     <numFmt numFmtId="181" formatCode="0.000000"/>
+    <numFmt numFmtId="182" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="183" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -2942,7 +2964,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
@@ -2983,78 +3005,20 @@
     <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="超連結" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="210">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="205">
     <dxf>
       <font>
         <condense val="0"/>
@@ -5853,12 +5817,12 @@
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="cellIs" dxfId="206" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7 D9">
-    <cfRule type="cellIs" dxfId="205" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7890,7 +7854,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -7899,8 +7863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D522"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9179,12 +9143,12 @@
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
   <conditionalFormatting sqref="D3:D5">
-    <cfRule type="cellIs" dxfId="204" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7 D9">
-    <cfRule type="cellIs" dxfId="203" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9223,17 +9187,17 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
     </row>
     <row r="3" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
@@ -10083,7 +10047,7 @@
       </c>
       <c r="B92" s="9">
         <f ca="1">RAND()*100</f>
-        <v>89.848801093555792</v>
+        <v>76.878089544695001</v>
       </c>
       <c r="C92" t="s">
         <v>69</v>
@@ -10101,7 +10065,7 @@
       </c>
       <c r="B94">
         <f ca="1">RANDBETWEEN(1,100)</f>
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="C94" t="s">
         <v>69</v>
@@ -10983,7 +10947,7 @@
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <conditionalFormatting sqref="D4 D7 D11 D13 D15 D17 D19 D21 D23 D25:D27 D29 D31 D33 D35 D37 D39 D41 D43 D45 D47 D53 D51 D49 D59 D63 D71 D75 D73 D79 D81 D83 D88:D90 D92 D96 D98:D100 D102 D104:D105 D111 D113 D115 D94 D117 D119 D121 D127 D129 D135 D145 D150 D153 D162 D171 D180 D182 D184 D9 D77 D186">
-    <cfRule type="cellIs" dxfId="202" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="14" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11194,7 +11158,7 @@
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
   <conditionalFormatting sqref="D4 D6 D8 D11 D14 D16 D18">
-    <cfRule type="cellIs" dxfId="201" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11207,7 +11171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D223"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -11346,7 +11310,7 @@
       <c r="A13" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B13" s="21" t="str">
+      <c r="B13" s="39" t="str">
         <f>DOLLAR(B14,2)</f>
         <v>$1,234.57</v>
       </c>
@@ -12375,12 +12339,12 @@
   </sortState>
   <phoneticPr fontId="12" type="noConversion"/>
   <conditionalFormatting sqref="D3:D73">
-    <cfRule type="cellIs" dxfId="200" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="198" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12809,17 +12773,17 @@
       <c r="A45" s="1"/>
     </row>
     <row r="46" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="38" t="s">
+      <c r="A46" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="B46" s="39" t="str">
+      <c r="B46" s="38" t="str">
         <f ca="1">INFO("release")</f>
         <v>14.0</v>
       </c>
-      <c r="C46" s="37" t="s">
+      <c r="C46" s="36" t="s">
         <v>395</v>
       </c>
-      <c r="D46" s="37" t="s">
+      <c r="D46" s="36" t="s">
         <v>457</v>
       </c>
     </row>
@@ -13811,7 +13775,7 @@
       </c>
       <c r="B34" s="20">
         <f ca="1">NOW()</f>
-        <v>41535.482294791669</v>
+        <v>41542.43128553241</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
@@ -13882,7 +13846,7 @@
       </c>
       <c r="B42" s="19">
         <f ca="1">TODAY()</f>
-        <v>41535</v>
+        <v>41542</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
@@ -16891,8 +16855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M623"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D170" sqref="D170"/>
+    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
+      <selection activeCell="E204" sqref="E204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -19693,11 +19657,44 @@
     <row r="201" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A201" s="1"/>
     </row>
+    <row r="202" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A202" s="37" t="s">
+        <v>259</v>
+      </c>
+      <c r="B202" s="22">
+        <f>GAMMADIST(10, 9,2, TRUE)</f>
+        <v>6.8093634721848553E-2</v>
+      </c>
+      <c r="C202" s="40">
+        <v>6.8093634721848553E-2</v>
+      </c>
+      <c r="D202" t="s">
+        <v>460</v>
+      </c>
+      <c r="E202" t="s">
+        <v>461</v>
+      </c>
+    </row>
     <row r="203" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A203" s="1"/>
     </row>
     <row r="204" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A204" s="1"/>
+      <c r="A204" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B204" s="22">
+        <f>TDIST(1.959999,60,1)</f>
+        <v>2.7322524716226902E-2</v>
+      </c>
+      <c r="C204" s="40">
+        <v>2.7322524716226902E-2</v>
+      </c>
+      <c r="D204" t="s">
+        <v>463</v>
+      </c>
+      <c r="E204" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="205" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A205" s="1"/>

</xml_diff>